<commit_message>
code and files for consistency and form
</commit_message>
<xml_diff>
--- a/cleaned all season/allrounderset_ipl.xlsx
+++ b/cleaned all season/allrounderset_ipl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/Dataset_Final/cleaned all season/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/cricket-squad-selection/cleaned all season/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C04D7-EA77-8D4A-97C6-A5D225087DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6D3CE3-048D-E740-B44D-F06CD8AC9FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>Player</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>2024-2024</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Abdul Samad</t>
@@ -683,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AE32" sqref="AE32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -797,15 +794,15 @@
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="2">
         <v>50</v>
@@ -888,10 +885,10 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>63</v>
@@ -974,10 +971,10 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>127</v>
@@ -1060,10 +1057,10 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>150</v>
@@ -1146,10 +1143,10 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="2">
         <v>10</v>
@@ -1232,10 +1229,10 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C7" s="2">
         <v>11</v>
@@ -1318,7 +1315,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -1404,7 +1401,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>27</v>
@@ -1490,10 +1487,10 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C10" s="2">
         <v>118</v>
@@ -1576,10 +1573,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2">
         <v>134</v>
@@ -1662,10 +1659,10 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2">
         <v>41</v>
@@ -1748,10 +1745,10 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2">
         <v>137</v>
@@ -1834,10 +1831,10 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2">
         <v>106</v>
@@ -1920,10 +1917,10 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C15" s="2">
         <v>20</v>
@@ -2006,10 +2003,10 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2">
         <v>15</v>
@@ -2092,10 +2089,10 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C17" s="2">
         <v>127</v>
@@ -2178,10 +2175,10 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C18" s="2">
         <v>12</v>
@@ -2264,10 +2261,10 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2">
         <v>39</v>
@@ -2350,10 +2347,10 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="C20" s="2">
         <v>21</v>
@@ -2436,10 +2433,10 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2">
         <v>40</v>
@@ -2498,14 +2495,14 @@
       <c r="U21" s="2">
         <v>0</v>
       </c>
-      <c r="V21" s="2" t="s">
-        <v>30</v>
+      <c r="V21" s="2">
+        <v>100</v>
       </c>
       <c r="W21" s="2">
         <v>7.5</v>
       </c>
-      <c r="X21" s="2" t="s">
-        <v>30</v>
+      <c r="X21" s="2">
+        <v>100</v>
       </c>
       <c r="Y21" s="2">
         <v>0</v>
@@ -2522,10 +2519,10 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2">
         <v>18</v>
@@ -2608,10 +2605,10 @@
     </row>
     <row r="23" spans="1:38" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2">
         <v>40</v>
@@ -2694,10 +2691,10 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2">
         <v>67</v>
@@ -2780,10 +2777,10 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2">
         <v>96</v>
@@ -2866,10 +2863,10 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C26" s="2">
         <v>42</v>
@@ -2952,10 +2949,10 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="2">
         <v>107</v>
@@ -3038,7 +3035,7 @@
     </row>
     <row r="28" spans="1:38" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
@@ -3100,14 +3097,14 @@
       <c r="U28" s="2">
         <v>0</v>
       </c>
-      <c r="V28" s="2" t="s">
-        <v>30</v>
+      <c r="V28" s="2">
+        <v>100</v>
       </c>
       <c r="W28" s="2">
         <v>11.78</v>
       </c>
-      <c r="X28" s="2" t="s">
-        <v>30</v>
+      <c r="X28" s="2">
+        <v>100</v>
       </c>
       <c r="Y28" s="2">
         <v>0</v>
@@ -3125,7 +3122,7 @@
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>27</v>
@@ -3187,14 +3184,14 @@
       <c r="U29" s="2">
         <v>0</v>
       </c>
-      <c r="V29" s="2" t="s">
-        <v>30</v>
+      <c r="V29" s="2">
+        <v>100</v>
       </c>
       <c r="W29" s="2">
         <v>7.63</v>
       </c>
-      <c r="X29" s="2" t="s">
-        <v>30</v>
+      <c r="X29" s="2">
+        <v>100</v>
       </c>
       <c r="Y29" s="2">
         <v>0</v>
@@ -3211,10 +3208,10 @@
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C30" s="2">
         <v>4</v>
@@ -3297,10 +3294,10 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2">
         <v>58</v>
@@ -3383,10 +3380,10 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C32" s="2">
         <v>212</v>
@@ -3469,10 +3466,10 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2">
         <v>70</v>
@@ -3555,7 +3552,7 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>29</v>
@@ -3617,14 +3614,14 @@
       <c r="U34" s="2">
         <v>0</v>
       </c>
-      <c r="V34" s="2" t="s">
-        <v>30</v>
+      <c r="V34" s="2">
+        <v>100</v>
       </c>
       <c r="W34" s="2">
         <v>3.5</v>
       </c>
-      <c r="X34" s="2" t="s">
-        <v>30</v>
+      <c r="X34" s="2">
+        <v>100</v>
       </c>
       <c r="Y34" s="2">
         <v>0</v>
@@ -3641,7 +3638,7 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>27</v>
@@ -3727,7 +3724,7 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>27</v>
@@ -3813,10 +3810,10 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="2">
         <v>93</v>
@@ -3899,10 +3896,10 @@
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C38" s="2">
         <v>240</v>
@@ -3985,7 +3982,7 @@
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>27</v>
@@ -4071,10 +4068,10 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="2">
         <v>65</v>
@@ -4157,10 +4154,10 @@
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="2">
         <v>55</v>
@@ -4243,7 +4240,7 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>27</v>
@@ -4329,10 +4326,10 @@
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="2">
         <v>59</v>
@@ -4415,10 +4412,10 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="2">
         <v>14</v>
@@ -4501,10 +4498,10 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45" s="2">
         <v>72</v>
@@ -4587,10 +4584,10 @@
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C46" s="2">
         <v>60</v>
@@ -4673,7 +4670,7 @@
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>29</v>
@@ -4759,10 +4756,10 @@
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="2">
         <v>5</v>

</xml_diff>